<commit_message>
day5 - working with props
</commit_message>
<xml_diff>
--- a/diem_danh_giay_29_06_23_11_17_11.xlsx
+++ b/diem_danh_giay_29_06_23_11_17_11.xlsx
@@ -362,11 +362,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -396,11 +397,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -411,32 +418,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,6 +429,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,14 +450,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -496,10 +480,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -510,13 +495,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -525,21 +535,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -556,6 +557,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -568,25 +593,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,7 +629,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,13 +647,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,43 +683,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,13 +719,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,43 +737,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,11 +766,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,6 +786,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -809,6 +831,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -832,185 +863,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1037,6 +1038,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1425,8 +1427,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1568,7 +1570,9 @@
       <c r="E5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="12">
+        <v>45122</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1606,7 +1610,9 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1644,7 +1650,9 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1682,7 +1690,9 @@
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1720,7 +1730,9 @@
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1758,7 +1770,9 @@
       <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1796,7 +1810,9 @@
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1834,7 +1850,9 @@
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1872,7 +1890,9 @@
       <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1910,7 +1930,9 @@
       <c r="E14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1948,7 +1970,9 @@
       <c r="E15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1986,7 +2010,9 @@
       <c r="E16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2024,7 +2050,9 @@
       <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2062,7 +2090,9 @@
       <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2100,7 +2130,9 @@
       <c r="E19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2138,7 +2170,9 @@
       <c r="E20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2176,7 +2210,9 @@
       <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2214,7 +2250,9 @@
       <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2252,7 +2290,9 @@
       <c r="E23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2290,7 +2330,9 @@
       <c r="E24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2328,7 +2370,9 @@
       <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2366,7 +2410,9 @@
       <c r="E26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2404,7 +2450,9 @@
       <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2442,7 +2490,9 @@
       <c r="E28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2480,7 +2530,9 @@
       <c r="E29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2518,7 +2570,9 @@
       <c r="E30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2556,7 +2610,9 @@
       <c r="E31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2594,7 +2650,9 @@
       <c r="E32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2632,7 +2690,9 @@
       <c r="E33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2670,7 +2730,9 @@
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2708,7 +2770,9 @@
       <c r="E35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2746,7 +2810,9 @@
       <c r="E36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2784,7 +2850,9 @@
       <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>

</xml_diff>